<commit_message>
Replaced SOT23-6 by SC70-6 foot print for IC9 Moved copyright info away from trace fixed font of silk screen
</commit_message>
<xml_diff>
--- a/mainboardv1.2-plc.xlsx
+++ b/mainboardv1.2-plc.xlsx
@@ -525,10 +525,10 @@
   <dimension ref="A1:F128"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E64" activeCellId="0" sqref="E64"/>
+      <selection pane="topLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
@@ -1621,7 +1621,7 @@
         <v>69</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>55.3125</v>
+        <v>55.9375</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>25.3125</v>

</xml_diff>